<commit_message>
replaced FIRST baseline with MAXDIV
</commit_message>
<xml_diff>
--- a/results/allOct9pacman5trajectories_filtered.xlsx
+++ b/results/allOct9pacman5trajectories_filtered.xlsx
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
     <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
 </workbook>
@@ -10630,7 +10630,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -45584,7 +45584,7 @@
   <dimension ref="A1:H841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45619,7 +45619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -45760,7 +45760,7 @@
         <v>1507549805402</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -45878,7 +45878,7 @@
         <v>1507549850245</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -45927,7 +45927,7 @@
         <v>1507549896882</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -46183,7 +46183,7 @@
         <v>1507549982714</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -46301,7 +46301,7 @@
         <v>1507550003257</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -46511,7 +46511,7 @@
         <v>1507550057106</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -46606,7 +46606,7 @@
         <v>1507550111521</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -46724,7 +46724,7 @@
         <v>1507550171129</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -46914,7 +46914,7 @@
         <v>1507550215413</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -47101,7 +47101,7 @@
         <v>1507550274265</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -47314,7 +47314,7 @@
         <v>1507550307191</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>4</v>
       </c>
@@ -47458,7 +47458,7 @@
         <v>1507550348537</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>93</v>
       </c>
@@ -47599,7 +47599,7 @@
         <v>1507550391630</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>4</v>
       </c>
@@ -47694,7 +47694,7 @@
         <v>1507550392648</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>61</v>
       </c>
@@ -47789,7 +47789,7 @@
         <v>1507550431046</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -47953,7 +47953,7 @@
         <v>1507550466219</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>61</v>
       </c>
@@ -48143,7 +48143,7 @@
         <v>1507550499426</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>93</v>
       </c>
@@ -48382,7 +48382,7 @@
         <v>1507550576888</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>93</v>
       </c>
@@ -48756,7 +48756,7 @@
         <v>1507550723142</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>115</v>
       </c>
@@ -48805,7 +48805,7 @@
         <v>1507550735109</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>61</v>
       </c>
@@ -48946,7 +48946,7 @@
         <v>1507550767533</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>93</v>
       </c>
@@ -49064,7 +49064,7 @@
         <v>1507550832080</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>93</v>
       </c>
@@ -49231,7 +49231,7 @@
         <v>1507550909862</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>61</v>
       </c>
@@ -49418,7 +49418,7 @@
         <v>1507550971022</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>61</v>
       </c>
@@ -49556,7 +49556,7 @@
         <v>1507551093131</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>162</v>
       </c>
@@ -49674,7 +49674,7 @@
         <v>1507551187271</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>115</v>
       </c>
@@ -49746,7 +49746,7 @@
         <v>1507551297465</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -49841,7 +49841,7 @@
         <v>1507551321882</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>162</v>
       </c>
@@ -49959,7 +49959,7 @@
         <v>1507551350753</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>177</v>
       </c>
@@ -50054,7 +50054,7 @@
         <v>1507551356951</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>115</v>
       </c>
@@ -50267,7 +50267,7 @@
         <v>1507551443085</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>162</v>
       </c>
@@ -50362,7 +50362,7 @@
         <v>1507551466495</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>177</v>
       </c>
@@ -50434,7 +50434,7 @@
         <v>1507551531469</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>177</v>
       </c>
@@ -50742,7 +50742,7 @@
         <v>1507551600682</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>162</v>
       </c>
@@ -51113,7 +51113,7 @@
         <v>1507551658515</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>162</v>
       </c>
@@ -51208,7 +51208,7 @@
         <v>1507551680942</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>177</v>
       </c>
@@ -51303,7 +51303,7 @@
         <v>1507551660291</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>157</v>
       </c>
@@ -51542,7 +51542,7 @@
         <v>1507551767487</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>201</v>
       </c>
@@ -51683,7 +51683,7 @@
         <v>1507551782206</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>162</v>
       </c>
@@ -51847,7 +51847,7 @@
         <v>1507551829513</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>201</v>
       </c>
@@ -51919,7 +51919,7 @@
         <v>1507551829522</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>211</v>
       </c>
@@ -52103,7 +52103,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>177</v>
       </c>
@@ -52270,7 +52270,7 @@
         <v>1507551894382</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>209</v>
       </c>
@@ -52388,7 +52388,7 @@
         <v>1507551902505</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>211</v>
       </c>
@@ -52621,7 +52621,7 @@
         <v>1507551970424</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>115</v>
       </c>
@@ -52811,7 +52811,7 @@
         <v>1507551982149</v>
       </c>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>218</v>
       </c>
@@ -53119,7 +53119,7 @@
         <v>1507551948839</v>
       </c>
     </row>
-    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>157</v>
       </c>
@@ -53214,7 +53214,7 @@
         <v>1507552016618</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>201</v>
       </c>
@@ -53283,7 +53283,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>218</v>
       </c>
@@ -53378,7 +53378,7 @@
         <v>1507552064493</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>201</v>
       </c>
@@ -53473,7 +53473,7 @@
         <v>1507552075058</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>209</v>
       </c>
@@ -53706,7 +53706,7 @@
         <v>1507552111712</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>115</v>
       </c>
@@ -53827,7 +53827,7 @@
         <v>1507552060057</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>201</v>
       </c>
@@ -53922,7 +53922,7 @@
         <v>1507552117945</v>
       </c>
     </row>
-    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>209</v>
       </c>
@@ -54086,7 +54086,7 @@
         <v>1507552167057</v>
       </c>
     </row>
-    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>201</v>
       </c>
@@ -54181,7 +54181,7 @@
         <v>1507552176840</v>
       </c>
     </row>
-    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>211</v>
       </c>
@@ -54319,7 +54319,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>218</v>
       </c>
@@ -54532,7 +54532,7 @@
         <v>1507552240861</v>
       </c>
     </row>
-    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>211</v>
       </c>
@@ -54834,7 +54834,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>157</v>
       </c>
@@ -54860,7 +54860,7 @@
         <v>1507552229621</v>
       </c>
     </row>
-    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>209</v>
       </c>
@@ -55001,7 +55001,7 @@
         <v>1507552295093</v>
       </c>
     </row>
-    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>218</v>
       </c>
@@ -55139,7 +55139,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>115</v>
       </c>
@@ -55349,7 +55349,7 @@
         <v>1507552361729</v>
       </c>
     </row>
-    <row r="415" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>256</v>
       </c>
@@ -55654,7 +55654,7 @@
         <v>1507552394880</v>
       </c>
     </row>
-    <row r="428" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>211</v>
       </c>
@@ -55841,7 +55841,7 @@
         <v>1507552415890</v>
       </c>
     </row>
-    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>218</v>
       </c>
@@ -55959,7 +55959,7 @@
         <v>1507552364312</v>
       </c>
     </row>
-    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>157</v>
       </c>
@@ -56126,7 +56126,7 @@
         <v>1507552429784</v>
       </c>
     </row>
-    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>256</v>
       </c>
@@ -56195,7 +56195,7 @@
         <v>1507552440145</v>
       </c>
     </row>
-    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>209</v>
       </c>
@@ -56359,7 +56359,7 @@
         <v>1507552458116</v>
       </c>
     </row>
-    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>256</v>
       </c>
@@ -56474,7 +56474,7 @@
         <v>1507552465524</v>
       </c>
     </row>
-    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>211</v>
       </c>
@@ -56569,7 +56569,7 @@
         <v>1507552469403</v>
       </c>
     </row>
-    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>218</v>
       </c>
@@ -56891,7 +56891,7 @@
         <v>1507552496100</v>
       </c>
     </row>
-    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>256</v>
       </c>
@@ -56940,7 +56940,7 @@
         <v>1507552513473</v>
       </c>
     </row>
-    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>209</v>
       </c>
@@ -57124,7 +57124,7 @@
         <v>1507552516178</v>
       </c>
     </row>
-    <row r="491" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>256</v>
       </c>
@@ -57216,7 +57216,7 @@
         <v>1507552537726</v>
       </c>
     </row>
-    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>256</v>
       </c>
@@ -57383,7 +57383,7 @@
         <v>1507552732901</v>
       </c>
     </row>
-    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>157</v>
       </c>
@@ -57524,7 +57524,7 @@
         <v>1507552871059</v>
       </c>
     </row>
-    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>157</v>
       </c>
@@ -57645,7 +57645,7 @@
         <v>1507553491986</v>
       </c>
     </row>
-    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>301</v>
       </c>
@@ -57809,7 +57809,7 @@
         <v>1507553752954</v>
       </c>
     </row>
-    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>301</v>
       </c>
@@ -57904,7 +57904,7 @@
         <v>1507553807846</v>
       </c>
     </row>
-    <row r="524" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>301</v>
       </c>
@@ -57953,7 +57953,7 @@
         <v>1507553807841</v>
       </c>
     </row>
-    <row r="526" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>301</v>
       </c>
@@ -58117,7 +58117,7 @@
         <v>1507553863652</v>
       </c>
     </row>
-    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>301</v>
       </c>
@@ -58330,7 +58330,7 @@
         <v>1507553914552</v>
       </c>
     </row>
-    <row r="542" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>301</v>
       </c>
@@ -58402,7 +58402,7 @@
         <v>1507553946132</v>
       </c>
     </row>
-    <row r="545" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>194</v>
       </c>
@@ -58759,7 +58759,7 @@
         <v>1507554000091</v>
       </c>
     </row>
-    <row r="560" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>194</v>
       </c>
@@ -58923,7 +58923,7 @@
         <v>1507554088059</v>
       </c>
     </row>
-    <row r="567" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
         <v>194</v>
       </c>
@@ -58995,7 +58995,7 @@
         <v>1507554124875</v>
       </c>
     </row>
-    <row r="570" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>194</v>
       </c>
@@ -59133,7 +59133,7 @@
         <v>1507554171164</v>
       </c>
     </row>
-    <row r="576" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
         <v>194</v>
       </c>
@@ -59366,7 +59366,7 @@
         <v>1507554253809</v>
       </c>
     </row>
-    <row r="586" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>194</v>
       </c>
@@ -59458,7 +59458,7 @@
         <v>1507543938041</v>
       </c>
     </row>
-    <row r="590" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
         <v>341</v>
       </c>
@@ -59743,7 +59743,7 @@
         <v>1507544028656</v>
       </c>
     </row>
-    <row r="602" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
         <v>339</v>
       </c>
@@ -59884,7 +59884,7 @@
         <v>1507544029036</v>
       </c>
     </row>
-    <row r="608" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
         <v>341</v>
       </c>
@@ -59930,7 +59930,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="610" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>339</v>
       </c>
@@ -60114,7 +60114,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="618" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>341</v>
       </c>
@@ -60186,7 +60186,7 @@
         <v>1507544166186</v>
       </c>
     </row>
-    <row r="621" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A621" t="s">
         <v>339</v>
       </c>
@@ -60281,7 +60281,7 @@
         <v>1507544159324</v>
       </c>
     </row>
-    <row r="625" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A625" t="s">
         <v>341</v>
       </c>
@@ -60439,7 +60439,7 @@
         <v>1507544222677</v>
       </c>
     </row>
-    <row r="632" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A632" t="s">
         <v>341</v>
       </c>
@@ -60534,7 +60534,7 @@
         <v>1507544232787</v>
       </c>
     </row>
-    <row r="636" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
         <v>339</v>
       </c>
@@ -60626,7 +60626,7 @@
         <v>1507544287964</v>
       </c>
     </row>
-    <row r="640" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A640" t="s">
         <v>341</v>
       </c>
@@ -60721,7 +60721,7 @@
         <v>1507544325385</v>
       </c>
     </row>
-    <row r="644" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
         <v>339</v>
       </c>
@@ -61193,7 +61193,7 @@
         <v>1507544554234</v>
       </c>
     </row>
-    <row r="664" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A664" t="s">
         <v>339</v>
       </c>
@@ -61288,7 +61288,7 @@
         <v>1507544731557</v>
       </c>
     </row>
-    <row r="668" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A668" t="s">
         <v>343</v>
       </c>
@@ -61409,7 +61409,7 @@
         <v>1507544776925</v>
       </c>
     </row>
-    <row r="673" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A673" t="s">
         <v>343</v>
       </c>
@@ -61573,7 +61573,7 @@
         <v>1507544956472</v>
       </c>
     </row>
-    <row r="680" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
         <v>343</v>
       </c>
@@ -61645,7 +61645,7 @@
         <v>1507545121228</v>
       </c>
     </row>
-    <row r="683" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>343</v>
       </c>
@@ -61763,7 +61763,7 @@
         <v>1507545210214</v>
       </c>
     </row>
-    <row r="688" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
         <v>373</v>
       </c>
@@ -62166,7 +62166,7 @@
         <v>1507545367999</v>
       </c>
     </row>
-    <row r="705" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
         <v>373</v>
       </c>
@@ -62261,7 +62261,7 @@
         <v>1507545335265</v>
       </c>
     </row>
-    <row r="709" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
         <v>343</v>
       </c>
@@ -62379,7 +62379,7 @@
         <v>1507545424811</v>
       </c>
     </row>
-    <row r="714" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
         <v>373</v>
       </c>
@@ -62451,7 +62451,7 @@
         <v>1507545424812</v>
       </c>
     </row>
-    <row r="717" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
         <v>343</v>
       </c>
@@ -62592,7 +62592,7 @@
         <v>1507545498654</v>
       </c>
     </row>
-    <row r="723" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
         <v>373</v>
       </c>
@@ -62759,7 +62759,7 @@
         <v>1507545564115</v>
       </c>
     </row>
-    <row r="730" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
         <v>373</v>
       </c>
@@ -62877,7 +62877,7 @@
         <v>1507545627855</v>
       </c>
     </row>
-    <row r="735" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
         <v>373</v>
       </c>
@@ -63090,7 +63090,7 @@
         <v>1507545776395</v>
       </c>
     </row>
-    <row r="744" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
         <v>385</v>
       </c>
@@ -63231,7 +63231,7 @@
         <v>1507545927993</v>
       </c>
     </row>
-    <row r="750" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
         <v>385</v>
       </c>
@@ -63611,7 +63611,7 @@
         <v>1507546205310</v>
       </c>
     </row>
-    <row r="766" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="766" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
         <v>385</v>
       </c>
@@ -63706,7 +63706,7 @@
         <v>1507546293977</v>
       </c>
     </row>
-    <row r="770" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>385</v>
       </c>
@@ -63801,7 +63801,7 @@
         <v>1507546404348</v>
       </c>
     </row>
-    <row r="774" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
         <v>385</v>
       </c>
@@ -63896,7 +63896,7 @@
         <v>1507546474976</v>
       </c>
     </row>
-    <row r="778" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
         <v>385</v>
       </c>
@@ -65376,13 +65376,6 @@
     <filterColumn colId="1">
       <filters>
         <filter val="correct"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="merged5f400"/>
-        <filter val="merged5m400"/>
-        <filter val="merged5r400"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -67642,7 +67635,7 @@
         <v>2</v>
       </c>
       <c r="I66">
-        <f t="shared" ref="I66:I97" si="2">IF(E66="m",8-H66,H66)</f>
+        <f t="shared" ref="I66:I81" si="2">IF(E66="m",8-H66,H66)</f>
         <v>6</v>
       </c>
       <c r="J66">

</xml_diff>